<commit_message>
add spare parts, working with 1 position
</commit_message>
<xml_diff>
--- a/eq_log/general equipment log.xlsx
+++ b/eq_log/general equipment log.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
   <si>
     <t>дата</t>
   </si>
@@ -395,6 +395,39 @@
   </si>
   <si>
     <t>246</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>248</t>
+  </si>
+  <si>
+    <t>1300</t>
+  </si>
+  <si>
+    <t>1301</t>
+  </si>
+  <si>
+    <t>1302</t>
+  </si>
+  <si>
+    <t>1303</t>
+  </si>
+  <si>
+    <t>1304</t>
+  </si>
+  <si>
+    <t>1305</t>
+  </si>
+  <si>
+    <t>1306</t>
+  </si>
+  <si>
+    <t>1307</t>
+  </si>
+  <si>
+    <t>1308</t>
   </si>
   <si>
     <t>**</t>
@@ -1065,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -2932,7 +2965,194 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
+        <v>118</v>
+      </c>
+      <c r="B110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>75</v>
+      </c>
+      <c r="D110" t="s">
+        <v>33</v>
+      </c>
+      <c r="E110" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>75</v>
+      </c>
+      <c r="D111" t="s">
+        <v>33</v>
+      </c>
+      <c r="E111" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>118</v>
+      </c>
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" t="s">
+        <v>75</v>
+      </c>
+      <c r="D112" t="s">
+        <v>33</v>
+      </c>
+      <c r="E112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
+        <v>75</v>
+      </c>
+      <c r="D113" t="s">
+        <v>33</v>
+      </c>
+      <c r="E113" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>118</v>
+      </c>
+      <c r="B114" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>33</v>
+      </c>
+      <c r="E114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>33</v>
+      </c>
+      <c r="E115" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>33</v>
+      </c>
+      <c r="E116" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>118</v>
+      </c>
+      <c r="B117" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" t="s">
+        <v>33</v>
+      </c>
+      <c r="E117" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>33</v>
+      </c>
+      <c r="E118" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>8</v>
+      </c>
+      <c r="C119" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" t="s">
+        <v>33</v>
+      </c>
+      <c r="E119" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>33</v>
+      </c>
+      <c r="E120" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2970,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -2982,10 +3202,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2993,7 +3213,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>9</v>
@@ -3002,10 +3222,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3013,7 +3233,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>9</v>
@@ -3022,7 +3242,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3030,7 +3250,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -3039,7 +3259,7 @@
         <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3047,7 +3267,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -3056,7 +3276,7 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3064,7 +3284,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -3081,7 +3301,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -3098,7 +3318,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3115,7 +3335,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3132,7 +3352,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -3141,7 +3361,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3149,7 +3369,7 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3158,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3166,7 +3386,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3175,7 +3395,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3183,7 +3403,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3192,7 +3412,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3200,7 +3420,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3209,7 +3429,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3217,16 +3437,16 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3234,16 +3454,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3251,7 +3471,7 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3260,7 +3480,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3268,7 +3488,7 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -3277,7 +3497,7 @@
         <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3285,7 +3505,7 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -3294,7 +3514,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3302,7 +3522,7 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -3311,7 +3531,7 @@
         <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3319,7 +3539,7 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -3328,7 +3548,7 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3336,7 +3556,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -3345,7 +3565,7 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3353,7 +3573,7 @@
         <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -3362,7 +3582,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3370,7 +3590,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -3379,7 +3599,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3387,7 +3607,7 @@
         <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -3396,7 +3616,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3404,7 +3624,7 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -3413,7 +3633,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3421,7 +3641,7 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -3430,7 +3650,7 @@
         <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3438,7 +3658,7 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -3447,7 +3667,7 @@
         <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3455,7 +3675,7 @@
         <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -3464,7 +3684,7 @@
         <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3472,7 +3692,7 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -3481,12 +3701,12 @@
         <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3524,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -3536,10 +3756,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3547,7 +3767,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -3564,7 +3784,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>9</v>
@@ -3581,10 +3801,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -3598,10 +3818,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -3615,7 +3835,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -3632,7 +3852,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -3649,7 +3869,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3666,7 +3886,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3683,7 +3903,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -3700,7 +3920,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3717,7 +3937,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3734,7 +3954,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3743,7 +3963,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3751,7 +3971,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3760,7 +3980,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3768,7 +3988,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3777,7 +3997,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3785,7 +4005,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -3794,7 +4014,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -3802,7 +4022,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -3811,7 +4031,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -3819,7 +4039,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -3828,7 +4048,7 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -3836,7 +4056,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -3845,7 +4065,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3853,7 +4073,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -3862,7 +4082,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3870,7 +4090,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -3879,7 +4099,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3887,7 +4107,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -3896,7 +4116,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3904,7 +4124,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -3913,7 +4133,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3921,7 +4141,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -3930,7 +4150,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3938,7 +4158,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -3947,7 +4167,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -3955,7 +4175,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -3964,7 +4184,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -3972,7 +4192,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -3981,7 +4201,7 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -3989,7 +4209,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -3998,7 +4218,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -4006,7 +4226,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -4015,7 +4235,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4023,7 +4243,7 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -4032,7 +4252,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4040,7 +4260,7 @@
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -4049,7 +4269,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -4057,7 +4277,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -4066,7 +4286,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -4074,7 +4294,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -4083,7 +4303,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -4091,7 +4311,7 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -4100,7 +4320,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -4108,7 +4328,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -4117,7 +4337,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -4125,7 +4345,7 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -4134,7 +4354,7 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -4142,7 +4362,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -4151,7 +4371,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -4159,7 +4379,7 @@
         <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -4176,7 +4396,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -4193,7 +4413,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -4202,7 +4422,7 @@
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -4210,7 +4430,7 @@
         <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -4219,12 +4439,12 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4262,7 +4482,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -4274,10 +4494,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4297,7 +4517,7 @@
         <v>99</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4317,15 +4537,15 @@
         <v>100</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
evrething is work, but not beautiful code
</commit_message>
<xml_diff>
--- a/eq_log/general equipment log.xlsx
+++ b/eq_log/general equipment log.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="219">
   <si>
     <t>дата</t>
   </si>
@@ -524,6 +524,57 @@
   </si>
   <si>
     <t>600014</t>
+  </si>
+  <si>
+    <t>06/03/2018</t>
+  </si>
+  <si>
+    <t>80001841</t>
+  </si>
+  <si>
+    <t>1201</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>1203</t>
+  </si>
+  <si>
+    <t>1204</t>
+  </si>
+  <si>
+    <t>1205</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>1207</t>
+  </si>
+  <si>
+    <t>1208</t>
+  </si>
+  <si>
+    <t>1209</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>1211</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>1220</t>
+  </si>
+  <si>
+    <t>Не вірна довжина проводу</t>
+  </si>
+  <si>
+    <t>1230</t>
   </si>
   <si>
     <t>номер зварки</t>
@@ -3167,7 +3218,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -3706,6 +3757,278 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>170</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3744,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -3759,7 +4082,7 @@
         <v>139</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3767,7 +4090,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>43</v>
@@ -3784,7 +4107,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>9</v>
@@ -3801,10 +4124,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -3818,10 +4141,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -3835,7 +4158,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -3852,7 +4175,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -3869,7 +4192,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3886,7 +4209,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3903,7 +4226,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -3920,7 +4243,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3937,7 +4260,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3954,7 +4277,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3963,7 +4286,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3971,7 +4294,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3980,7 +4303,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3988,7 +4311,7 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3997,7 +4320,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4005,7 +4328,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -4014,7 +4337,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4022,7 +4345,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
@@ -4031,7 +4354,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4039,7 +4362,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
@@ -4056,7 +4379,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -4065,7 +4388,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4073,7 +4396,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -4082,7 +4405,7 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4090,7 +4413,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -4099,7 +4422,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4107,7 +4430,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -4116,7 +4439,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4124,7 +4447,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -4133,7 +4456,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4141,7 +4464,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -4150,7 +4473,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4158,7 +4481,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -4167,7 +4490,7 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4175,7 +4498,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -4184,7 +4507,7 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -4192,7 +4515,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -4209,7 +4532,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -4226,7 +4549,7 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -4235,7 +4558,7 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4243,7 +4566,7 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -4252,7 +4575,7 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4260,7 +4583,7 @@
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -4269,7 +4592,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -4277,7 +4600,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -4286,7 +4609,7 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -4294,7 +4617,7 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -4303,7 +4626,7 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -4311,7 +4634,7 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -4320,7 +4643,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -4328,7 +4651,7 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -4337,7 +4660,7 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -4345,7 +4668,7 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -4354,7 +4677,7 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -4362,7 +4685,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -4371,7 +4694,7 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -4379,7 +4702,7 @@
         <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -4396,7 +4719,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -4413,7 +4736,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -4422,7 +4745,7 @@
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -4430,7 +4753,7 @@
         <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -4439,7 +4762,7 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -4482,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -4497,7 +4820,7 @@
         <v>139</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4517,7 +4840,7 @@
         <v>99</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4537,7 +4860,7 @@
         <v>100</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4545,7 +4868,7 @@
         <v>137</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>